<commit_message>
lesson #2 video record uploaded into YouTube
</commit_message>
<xml_diff>
--- a/src/main/java/az/et/_syllabus/course_details.xlsx
+++ b/src/main/java/az/et/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">№</t>
   </si>
@@ -39,6 +39,12 @@
   <si>
     <t xml:space="preserve">Part #1: https://youtu.be/SKviqOCYBC8
 Part #2: https://youtu.be/6WQnuH0XC6Q </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lesson #2 – Chapter [6-13]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/TOCrMo3FQuU </t>
   </si>
 </sst>
 </file>
@@ -306,10 +312,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ2"/>
+  <dimension ref="A1:AMJ3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -351,7 +357,21 @@
       <c r="AMI2" s="12"/>
       <c r="AMJ2" s="0"/>
     </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="9" t="n">
+        <v>44660</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" display="https://youtu.be/TOCrMo3FQuU"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>